<commit_message>
update for working with parsing inventory excel
parsing inventory excel via XLSX node addon
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam.bass.18\Downloads\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan.Smith.19\Documents\GitHub\smida_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
   <si>
     <t>shelf 0</t>
   </si>
@@ -88,6 +87,21 @@
   </si>
   <si>
     <t xml:space="preserve">Tetrix piece </t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>shelf</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -439,14 +453,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>

</xml_diff>